<commit_message>
for the love of good do OOP
</commit_message>
<xml_diff>
--- a/DataPipeline/TABLES/HealthiestCompanies.xlsx
+++ b/DataPipeline/TABLES/HealthiestCompanies.xlsx
@@ -3735,7 +3735,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>3.25017651687845</t>
+          <t>3.26887946369168</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -3760,7 +3760,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>34.4887473768001</t>
+          <t>33.8286092840581</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -5152,7 +5152,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>0.96649379703071</t>
+          <t>1.01993085214562</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -5162,17 +5162,17 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>1.882e+09</t>
+          <t>1.3987e+10</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.189112903225806</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1.75290697674419</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
@@ -5182,7 +5182,12 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>8.77090909090909</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>13.4816053511706</t>
         </is>
       </c>
     </row>
@@ -7828,17 +7833,17 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>1.36734274359326</t>
+          <t>1.09757862876694</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>1.67212553104015</t>
+          <t>1.47124621660745</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>5.78467125494344</t>
+          <t>3.11242698221738</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -7848,17 +7853,17 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>0.0530503113893508</t>
+          <t>0.250944746316048</t>
         </is>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>0.136554386750224</t>
+          <t>0.651108145741471</t>
         </is>
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>1.59987690241719</t>
+          <t>1.57043397540032</t>
         </is>
       </c>
       <c r="J135" t="inlineStr">
@@ -7868,7 +7873,7 @@
       </c>
       <c r="K135" t="inlineStr">
         <is>
-          <t>4.44567445674457</t>
+          <t>19.1647058823529</t>
         </is>
       </c>
     </row>
@@ -12630,7 +12635,7 @@
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>-1546978000</t>
+          <t>-1574949000</t>
         </is>
       </c>
       <c r="G221" t="inlineStr">
@@ -21425,7 +21430,7 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
@@ -25822,7 +25827,7 @@
       </c>
       <c r="E462" t="inlineStr">
         <is>
-          <t>25.0200885595518</t>
+          <t>25.020089446789</t>
         </is>
       </c>
       <c r="F462" t="inlineStr">
@@ -29994,7 +29999,7 @@
       </c>
       <c r="F538" t="inlineStr">
         <is>
-          <t>5.646e+09</t>
+          <t>5.764e+09</t>
         </is>
       </c>
       <c r="G538" t="inlineStr">
@@ -32261,42 +32266,42 @@
       </c>
       <c r="C579" t="inlineStr">
         <is>
-          <t>3.02469729891023</t>
+          <t>2.44045481083665</t>
         </is>
       </c>
       <c r="D579" t="inlineStr">
         <is>
-          <t>5.39893923283503</t>
+          <t>4.62443620053867</t>
         </is>
       </c>
       <c r="F579" t="inlineStr">
         <is>
-          <t>321543000</t>
+          <t>920698000</t>
         </is>
       </c>
       <c r="G579" t="inlineStr">
         <is>
-          <t>0.0341432527343263</t>
+          <t>0.0831103515368531</t>
         </is>
       </c>
       <c r="H579" t="inlineStr">
         <is>
-          <t>0.0774900675196707</t>
+          <t>0.18401707360004</t>
         </is>
       </c>
       <c r="I579" t="inlineStr">
         <is>
-          <t>1.25095556701686</t>
+          <t>1.20330093791647</t>
         </is>
       </c>
       <c r="J579" t="inlineStr">
         <is>
-          <t>9.05342366322527</t>
+          <t>20.4538633937914</t>
         </is>
       </c>
       <c r="K579" t="inlineStr">
         <is>
-          <t>3.59713898401826</t>
+          <t>11.0742979836146</t>
         </is>
       </c>
     </row>
@@ -32997,47 +33002,47 @@
       </c>
       <c r="C592" t="inlineStr">
         <is>
-          <t>6.39670826783022</t>
+          <t>8.03064901822101</t>
         </is>
       </c>
       <c r="D592" t="inlineStr">
         <is>
-          <t>6.47537617504572</t>
+          <t>8.41076420464114</t>
         </is>
       </c>
       <c r="E592" t="inlineStr">
         <is>
-          <t>24.074799370821</t>
+          <t>20.7773606655947</t>
         </is>
       </c>
       <c r="F592" t="inlineStr">
         <is>
-          <t>519584000</t>
+          <t>1011653000</t>
         </is>
       </c>
       <c r="G592" t="inlineStr">
         <is>
-          <t>0.0852410297867883</t>
+          <t>0.119896266782674</t>
         </is>
       </c>
       <c r="H592" t="inlineStr">
         <is>
-          <t>0.0888612636014147</t>
+          <t>0.120779339010774</t>
         </is>
       </c>
       <c r="I592" t="inlineStr">
         <is>
-          <t>0.0424705546575587</t>
+          <t>0.00736530212154428</t>
         </is>
       </c>
       <c r="J592" t="inlineStr">
         <is>
-          <t>46.3230142744549</t>
+          <t>62.8199206933713</t>
         </is>
       </c>
       <c r="K592" t="inlineStr">
         <is>
-          <t>42.0405951803332</t>
+          <t>1716.35795454545</t>
         </is>
       </c>
     </row>
@@ -39956,7 +39961,7 @@
       </c>
       <c r="B719" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C719" t="inlineStr">
@@ -40858,7 +40863,7 @@
       </c>
       <c r="F735" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1578636000</t>
         </is>
       </c>
       <c r="G735" t="inlineStr">
@@ -41128,7 +41133,7 @@
       </c>
       <c r="F740" t="inlineStr">
         <is>
-          <t>1586714188</t>
+          <t>1859629000</t>
         </is>
       </c>
       <c r="G740" t="inlineStr">
@@ -47716,17 +47721,17 @@
       </c>
       <c r="C859" t="inlineStr">
         <is>
-          <t>2.54397530606601</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D859" t="inlineStr">
         <is>
-          <t>0.629635701546517</t>
+          <t>0.648524656217272</t>
         </is>
       </c>
       <c r="E859" t="inlineStr">
         <is>
-          <t>22.7632122699558</t>
+          <t>18.4610413857687</t>
         </is>
       </c>
       <c r="F859" t="inlineStr">
@@ -47736,17 +47741,17 @@
       </c>
       <c r="G859" t="inlineStr">
         <is>
-          <t>0.0207838922190336</t>
+          <t>0.02944493207183</t>
         </is>
       </c>
       <c r="H859" t="inlineStr">
         <is>
-          <t>0.0608147908239264</t>
+          <t>0.0832512609823607</t>
         </is>
       </c>
       <c r="I859" t="inlineStr">
         <is>
-          <t>1.92605399330512</t>
+          <t>1.82735449276201</t>
         </is>
       </c>
       <c r="J859" t="inlineStr">
@@ -47756,7 +47761,7 @@
       </c>
       <c r="K859" t="inlineStr">
         <is>
-          <t>2.30682198105448</t>
+          <t>2.90169901159796</t>
         </is>
       </c>
     </row>
@@ -51927,7 +51932,7 @@
       </c>
       <c r="E937" t="inlineStr">
         <is>
-          <t>30.8004883099329</t>
+          <t>30.8004876479127</t>
         </is>
       </c>
       <c r="F937" t="inlineStr">

</xml_diff>